<commit_message>
demo lai file excel
</commit_message>
<xml_diff>
--- a/storage/app/private/demo_de_tai_du_an_cac_cap.xlsx
+++ b/storage/app/private/demo_de_tai_du_an_cac_cap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="33">
   <si>
     <t>chuyên ngành</t>
   </si>
@@ -82,6 +82,39 @@
   </si>
   <si>
     <t>this is test7</t>
+  </si>
+  <si>
+    <t>this is test8</t>
+  </si>
+  <si>
+    <t>this is test9</t>
+  </si>
+  <si>
+    <t>this is test10</t>
+  </si>
+  <si>
+    <t>this is test11</t>
+  </si>
+  <si>
+    <t>this is test12</t>
+  </si>
+  <si>
+    <t>this is test13</t>
+  </si>
+  <si>
+    <t>this is test14</t>
+  </si>
+  <si>
+    <t>this is test15</t>
+  </si>
+  <si>
+    <t>this is test16</t>
+  </si>
+  <si>
+    <t>this is test17</t>
+  </si>
+  <si>
+    <t>this is test18</t>
   </si>
 </sst>
 </file>
@@ -454,7 +487,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +841,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
         <v>1996</v>
@@ -846,7 +879,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>1996</v>
@@ -884,7 +917,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>1996</v>
@@ -922,7 +955,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>1996</v>
@@ -960,7 +993,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1">
         <v>1996</v>
@@ -998,7 +1031,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1">
         <v>1996</v>
@@ -1036,7 +1069,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>1996</v>
@@ -1074,7 +1107,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1">
         <v>1996</v>
@@ -1112,7 +1145,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1">
         <v>1996</v>
@@ -1150,7 +1183,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>1996</v>
@@ -1188,7 +1221,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1">
         <v>1996</v>

</xml_diff>